<commit_message>
Added screenshot capture and embeding
</commit_message>
<xml_diff>
--- a/Resources/testData.xlsx
+++ b/Resources/testData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8331" uniqueCount="364">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -2319,10 +2319,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B53" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C53" t="s">
         <v>307</v>
@@ -2333,10 +2333,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B54" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C54" t="s">
         <v>307</v>
@@ -2837,10 +2837,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>6</v>
+        <v>221</v>
       </c>
       <c r="B90" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C90" t="s">
         <v>307</v>
@@ -2851,10 +2851,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B91" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C91" t="s">
         <v>307</v>
@@ -2865,10 +2865,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>221</v>
+        <v>8</v>
       </c>
       <c r="B92" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C92" t="s">
         <v>307</v>
@@ -2935,10 +2935,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B97" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C97" t="s">
         <v>305</v>
@@ -2949,10 +2949,10 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="B98" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C98" t="s">
         <v>305</v>

</xml_diff>